<commit_message>
bf: add sch sth forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Burkina Faso/2024/oct/bf_2411_sch_ia_2_enrolement.xlsx
+++ b/SCH-STH/Impact assessments/Burkina Faso/2024/oct/bf_2411_sch_ia_2_enrolement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Burkina Faso\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Burkina Faso\2024\oct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FA0E95-A589-4553-B93B-C5CBF6D23C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DECABD6-F5E5-448E-A130-5C821161252B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="126">
   <si>
     <t>type</t>
   </si>
@@ -81,18 +81,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>p_drshp</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>p_district</t>
-  </si>
-  <si>
-    <t>District</t>
-  </si>
-  <si>
     <t>p_csps</t>
   </si>
   <si>
@@ -147,9 +135,6 @@
     <t xml:space="preserve">Le numéro complet de l'enquété </t>
   </si>
   <si>
-    <t>Code operateur_Codesite_numeroEnqueté</t>
-  </si>
-  <si>
     <t>${p_consent} = '1_oui'</t>
   </si>
   <si>
@@ -309,22 +294,131 @@
     <t>. &gt;= 5 and . &lt;= 15</t>
   </si>
   <si>
-    <t>bf_202403_sch_ia_2_enrolement</t>
-  </si>
-  <si>
-    <t>(BF - Mars 2024) impact schisto - 2. Formulaire Enrôlement</t>
+    <t>bf_2411_sch_ia_2_enrolement</t>
+  </si>
+  <si>
+    <t>(BF - Nov 2024) impact schisto - 2. Formulaire Enrôlement</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>p_commune</t>
+  </si>
+  <si>
+    <t>Commune</t>
+  </si>
+  <si>
+    <t>bind::db_get</t>
+  </si>
+  <si>
+    <t>bind::db_filter_by_col_1</t>
+  </si>
+  <si>
+    <t>col_1</t>
+  </si>
+  <si>
+    <t>col_2</t>
+  </si>
+  <si>
+    <t>col_3</t>
+  </si>
+  <si>
+    <t>col_4</t>
+  </si>
+  <si>
+    <t>col_5</t>
+  </si>
+  <si>
+    <t>col_6</t>
+  </si>
+  <si>
+    <t>bind::db_filter_by_col_2</t>
+  </si>
+  <si>
+    <t>bind::db_filter_by_col_3</t>
+  </si>
+  <si>
+    <t>bind::db_filter_by_col_4</t>
+  </si>
+  <si>
+    <t>bind::db_filter_by_col_5</t>
+  </si>
+  <si>
+    <t>${p_commune}</t>
+  </si>
+  <si>
+    <t>${p_ds}</t>
+  </si>
+  <si>
+    <t>p_ds</t>
+  </si>
+  <si>
+    <t>${p_csps}</t>
+  </si>
+  <si>
+    <t>${p_Ecole}</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>begin repeat</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>position(..)</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Enrôlement</t>
+  </si>
+  <si>
+    <t>bf_ia_e_2411</t>
+  </si>
+  <si>
+    <t>join(' ', ${p_Numero_Enquete_complet})</t>
+  </si>
+  <si>
+    <t>if (${C2} = 1,'',substring-after(${C1},${p_Numero_Enquete_complet}))</t>
+  </si>
+  <si>
+    <t>Cet identifiant a déjà été utilisé dans ce village.</t>
+  </si>
+  <si>
+    <t>end repeat</t>
+  </si>
+  <si>
+    <t>${p_Village}</t>
+  </si>
+  <si>
+    <t>not(selected(${C3}, ${p_Numero_Enquete_complet}))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="9">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -386,8 +480,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,8 +530,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFBE4D5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -442,50 +566,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -815,10 +989,13 @@
     <col min="11" max="11" width="41.140625" style="13" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="13"/>
     <col min="13" max="13" width="13.7109375" style="13" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="13"/>
+    <col min="14" max="14" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="29.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="18.75">
+    <row r="1" spans="1:20" s="7" customFormat="1" ht="18.75">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -861,8 +1038,26 @@
       <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="15.75">
+      <c r="O1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15.75">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
@@ -876,29 +1071,32 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75">
+    <row r="3" spans="1:20" ht="15.75">
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>20</v>
+        <v>109</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>92</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.75">
+      <c r="O3" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15.75">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>22</v>
+        <v>93</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>94</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -912,16 +1110,22 @@
       <c r="K4" s="14"/>
       <c r="L4" s="14"/>
       <c r="M4" s="14"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75">
+      <c r="O4" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15.75">
       <c r="A5" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -932,16 +1136,22 @@
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
       <c r="M5" s="15"/>
-    </row>
-    <row r="6" spans="1:14" s="8" customFormat="1" ht="15.75">
+      <c r="O5" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="8" customFormat="1" ht="15.75">
       <c r="A6" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -955,16 +1165,22 @@
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="12"/>
-    </row>
-    <row r="7" spans="1:14" s="8" customFormat="1" ht="15.75">
+      <c r="O6" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="8" customFormat="1" ht="15.75">
       <c r="A7" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -978,16 +1194,22 @@
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="12"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75">
+      <c r="O7" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="15.75">
       <c r="A8" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G8" s="14"/>
       <c r="I8" s="14"/>
@@ -997,216 +1219,340 @@
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="15"/>
-    </row>
-    <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="13" t="s">
+      <c r="O8" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="22" customFormat="1" ht="15.75">
+      <c r="A9" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+    </row>
+    <row r="10" spans="1:20" s="22" customFormat="1" ht="15.75">
+      <c r="A10" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="28"/>
+    </row>
+    <row r="11" spans="1:20" s="22" customFormat="1" ht="15.75">
+      <c r="A11" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+    </row>
+    <row r="12" spans="1:20" s="22" customFormat="1" ht="15.75">
+      <c r="A12" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+    </row>
+    <row r="13" spans="1:20" ht="15.75">
+      <c r="A13" s="14"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="15"/>
+      <c r="T13" s="19"/>
+    </row>
+    <row r="14" spans="1:20" ht="15.75">
+      <c r="A14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="15"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="C15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="F15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="15"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="14" t="s">
+      <c r="G15" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="13" t="s">
+      <c r="H15" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="45">
-      <c r="A11" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>42</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>55</v>
+    <row r="16" spans="1:20" ht="45">
+      <c r="A16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>122</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>38</v>
       </c>
       <c r="J16" s="13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="C23" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="13" t="s">
+    </row>
+    <row r="24" spans="1:14" customFormat="1">
+      <c r="A24" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="B25" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="14" t="s">
+    <row r="26" spans="1:14">
+      <c r="A26" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B26" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="14"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="14"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1230,7 +1576,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1239,101 +1585,101 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
         <v>71</v>
       </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="2" customFormat="1">
@@ -1341,24 +1687,24 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="2" customFormat="1">
@@ -1366,24 +1712,24 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="2" customFormat="1"/>
@@ -1453,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1465,24 +1811,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
         <v>90</v>
       </c>
-      <c r="B1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" t="s">
-        <v>95</v>
-      </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bf: update the form sch sth
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Burkina Faso/2024/oct/bf_2411_sch_ia_2_enrolement.xlsx
+++ b/SCH-STH/Impact assessments/Burkina Faso/2024/oct/bf_2411_sch_ia_2_enrolement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Burkina Faso\2024\oct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DECABD6-F5E5-448E-A130-5C821161252B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE42098-AAB4-4E16-8CEB-2D1C315BF184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -294,12 +294,6 @@
     <t>. &gt;= 5 and . &lt;= 15</t>
   </si>
   <si>
-    <t>bf_2411_sch_ia_2_enrolement</t>
-  </si>
-  <si>
-    <t>(BF - Nov 2024) impact schisto - 2. Formulaire Enrôlement</t>
-  </si>
-  <si>
     <t>DS</t>
   </si>
   <si>
@@ -381,9 +375,6 @@
     <t>Enrôlement</t>
   </si>
   <si>
-    <t>bf_ia_e_2411</t>
-  </si>
-  <si>
     <t>join(' ', ${p_Numero_Enquete_complet})</t>
   </si>
   <si>
@@ -400,18 +391,34 @@
   </si>
   <si>
     <t>not(selected(${C3}, ${p_Numero_Enquete_complet}))</t>
+  </si>
+  <si>
+    <t>bf_2411_sch_ia_2_enrolementv2</t>
+  </si>
+  <si>
+    <t>(BF - Nov 2024) impact schisto - 2. Formulaire Enrôlement V2</t>
+  </si>
+  <si>
+    <t>bf_ia_e_2411_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -585,82 +592,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,7 +979,7 @@
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1039,22 +1047,22 @@
         <v>13</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Q1" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75">
@@ -1076,16 +1084,16 @@
         <v>18</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>17</v>
       </c>
       <c r="O3" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75">
@@ -1093,10 +1101,10 @@
         <v>18</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -1111,10 +1119,10 @@
       <c r="L4" s="14"/>
       <c r="M4" s="14"/>
       <c r="O4" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="P4" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75">
@@ -1137,10 +1145,10 @@
       <c r="L5" s="14"/>
       <c r="M5" s="15"/>
       <c r="O5" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="8" customFormat="1" ht="15.75">
@@ -1166,10 +1174,10 @@
       <c r="L6" s="10"/>
       <c r="M6" s="12"/>
       <c r="O6" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:20" s="8" customFormat="1" ht="15.75">
@@ -1195,10 +1203,10 @@
       <c r="L7" s="10"/>
       <c r="M7" s="12"/>
       <c r="O7" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75">
@@ -1220,18 +1228,18 @@
       <c r="L8" s="14"/>
       <c r="M8" s="15"/>
       <c r="O8" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="22" customFormat="1" ht="15.75">
       <c r="A9" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -1240,7 +1248,7 @@
       <c r="G9"/>
       <c r="H9" s="21"/>
       <c r="I9" s="20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
@@ -1249,13 +1257,13 @@
     </row>
     <row r="10" spans="1:20" s="22" customFormat="1" ht="15.75">
       <c r="A10" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="23"/>
@@ -1271,10 +1279,10 @@
     </row>
     <row r="11" spans="1:20" s="22" customFormat="1" ht="15.75">
       <c r="A11" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -1283,7 +1291,7 @@
       <c r="G11"/>
       <c r="H11" s="21"/>
       <c r="I11" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
@@ -1292,10 +1300,10 @@
     </row>
     <row r="12" spans="1:20" s="22" customFormat="1" ht="15.75">
       <c r="A12" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -1304,7 +1312,7 @@
       <c r="G12"/>
       <c r="H12" s="21"/>
       <c r="I12" s="20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
@@ -1370,17 +1378,17 @@
       <c r="A16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="32" t="s">
-        <v>125</v>
+      <c r="F16" s="31" t="s">
+        <v>122</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H16" s="18" t="s">
         <v>37</v>
@@ -1515,22 +1523,22 @@
       </c>
     </row>
     <row r="24" spans="1:14" customFormat="1">
-      <c r="A24" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
+      <c r="A24" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="13" t="s">
@@ -1552,7 +1560,7 @@
       <c r="A29" s="14"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1805,29 +1813,30 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="58.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="1" max="1" width="58.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" style="33" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="33" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="33" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>